<commit_message>
Corrigindo a gramática e o First/Follow
</commit_message>
<xml_diff>
--- a/GramaticaCorrigida_FirstFollow_TabelaPreditiva.xlsx
+++ b/GramaticaCorrigida_FirstFollow_TabelaPreditiva.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas Tertuliano\Desktop\7º Semestre\Compiladores\Trabalho de Compiladores\TrabalhoPraticoCompiladores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{29705ECE-2C1B-41F7-A249-E56CDDE638CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7662EACF-1C7A-4E3B-86E3-019D08EE0699}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="11625" activeTab="1" xr2:uid="{45E39C20-C4C3-4463-802B-561D995510B5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="169">
   <si>
     <t>RECURSÃO E FATORAÇÃO A ESQUERDA</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">prog </t>
   </si>
   <si>
-    <t xml:space="preserve"> “program” “id” body </t>
-  </si>
-  <si>
     <t xml:space="preserve">body </t>
   </si>
   <si>
@@ -46,9 +43,6 @@
     <t>decl-list</t>
   </si>
   <si>
-    <t xml:space="preserve">decl “;” decl-list |  ε </t>
-  </si>
-  <si>
     <t>decl</t>
   </si>
   <si>
@@ -58,9 +52,6 @@
     <t>type</t>
   </si>
   <si>
-    <t xml:space="preserve"> “num” | “char” </t>
-  </si>
-  <si>
     <t>id-list</t>
   </si>
   <si>
@@ -70,21 +61,12 @@
     <t>id-list'</t>
   </si>
   <si>
-    <t>“,” id-list | ε</t>
-  </si>
-  <si>
     <t>stmt-list</t>
   </si>
   <si>
-    <t xml:space="preserve"> stmt “;” stmt-list | ε </t>
-  </si>
-  <si>
     <t>stmt</t>
   </si>
   <si>
-    <t xml:space="preserve">assign-stmt | if-stmt | while-stmt | read-stmt | write-stmt </t>
-  </si>
-  <si>
     <t>assign-stmt</t>
   </si>
   <si>
@@ -100,9 +82,6 @@
     <t>if-stmt'</t>
   </si>
   <si>
-    <t xml:space="preserve"> “else” “{“ stmt-list “}” | ε</t>
-  </si>
-  <si>
     <t>condition</t>
   </si>
   <si>
@@ -136,18 +115,12 @@
     <t>writable</t>
   </si>
   <si>
-    <t>simple-expr | “literal”</t>
-  </si>
-  <si>
     <t xml:space="preserve"> simple-expr  expression'</t>
   </si>
   <si>
     <t>expression'</t>
   </si>
   <si>
-    <t>relop simple-expr | ε</t>
-  </si>
-  <si>
     <t>simple-expr</t>
   </si>
   <si>
@@ -157,9 +130,6 @@
     <t>simple-expr'</t>
   </si>
   <si>
-    <t>addop term  simple-expr' | ε</t>
-  </si>
-  <si>
     <t>term</t>
   </si>
   <si>
@@ -169,45 +139,24 @@
     <t>term'</t>
   </si>
   <si>
-    <t>mulop factor-a  term' | ε</t>
-  </si>
-  <si>
     <t xml:space="preserve">factor-a </t>
   </si>
   <si>
-    <t xml:space="preserve"> factor | “not” factor</t>
-  </si>
-  <si>
     <t>factor</t>
   </si>
   <si>
-    <t xml:space="preserve"> “id” | constant | “(“ expression “)” </t>
-  </si>
-  <si>
     <t xml:space="preserve">relop </t>
   </si>
   <si>
-    <t xml:space="preserve"> “==” | “&gt;” | “&gt;=” | “&lt;” | “&lt;=” | “!=” </t>
-  </si>
-  <si>
     <t xml:space="preserve">addop </t>
   </si>
   <si>
-    <t xml:space="preserve"> “+” | “-” | “or” </t>
-  </si>
-  <si>
     <t xml:space="preserve">mulop </t>
   </si>
   <si>
-    <t xml:space="preserve"> “*” | “/” | “and” </t>
-  </si>
-  <si>
     <t xml:space="preserve">constant </t>
   </si>
   <si>
-    <t xml:space="preserve"> “num_const” | “char_const”</t>
-  </si>
-  <si>
     <t>GRAMÁTICA CORRIGIDA</t>
   </si>
   <si>
@@ -277,13 +226,7 @@
     <t>"==", "&gt;", "&gt;=", "&lt;", "&lt;=", "!=", ε</t>
   </si>
   <si>
-    <t>";", "==", "&gt;", "&gt;=", "&lt;", "&lt;=", "!=", )</t>
-  </si>
-  <si>
     <t>"+", "-", or, ε</t>
-  </si>
-  <si>
-    <t>"+", "-", or, ";", "==", "&gt;", "&gt;=", "&lt;", "&lt;=", "!=", )</t>
   </si>
   <si>
     <t>"*", "/", and, ε</t>
@@ -516,13 +459,1067 @@
   </si>
   <si>
     <t>Alunos:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “program” “id” body </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">decl-list “{“ stmt-list “}” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">decl “;” decl-list </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">|  ε </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> type id-list </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “num” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “char” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “id” id-list' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">“,” id-list </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| ε </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> stmt “;” stmt-list </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| ε </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">assign-stmt </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| if-stmt </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| while-stmt </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| read-stmt </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| write-stmt </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>17</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “id” “=” simple_expr </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “if” “(“ condition “)” “{“ stmt-list “}”  if-stmt' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “else” “{“ stmt-list “}” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| ε </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">expression </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">stmt-prefix “{“ stmt-list “}”  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">“while” “(“ condition “)” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “read” “id” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">“write” writable </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>26</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">simple-expr </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “literal” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>28</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> simple-expr  expression' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>29</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">relop simple-expr </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| ε </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>31</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">term simple-expr' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>32</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">addop term simple-expr' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>33</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| ε </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>34</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> factor-a  term' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>35</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mulop factor-a term' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>36</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| ε </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>37</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> factor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>38</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “not” factor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>39</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “id” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| constant </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>41</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “(“ expression “)” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>42</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “==” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>43</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “&gt;” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>44</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “&gt;=” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “&lt;” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>46</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “&lt;=” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>47</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “!=” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>48</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “+” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>49</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “-” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “or” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>51</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “*” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “/” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “and” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>54</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> “num_const” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">| “char_const” </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>56</t>
+    </r>
+  </si>
+  <si>
+    <t>num, char, {</t>
+  </si>
+  <si>
+    <t>";", "==", "&gt;", "&gt;=", "&lt;", "&lt;=", "!=", ")"</t>
+  </si>
+  <si>
+    <t>"+", "-", or, ";", "==", "&gt;", "&gt;=", "&lt;", "&lt;=", "!=", ")"</t>
+  </si>
+  <si>
+    <t>"*", "/", and, "+", "-", or, ";", "==", "&gt;", "&gt;=", "&lt;", "&lt;=", "!=", ")"</t>
+  </si>
+  <si>
+    <t>id, num_const, char_const, "(", not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“program” “id” body </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,6 +1563,14 @@
       <i/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -660,18 +1665,24 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -686,14 +1697,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1015,564 +2021,564 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6ACCDF-ECC4-4644-8B3C-8B75FF82EFD2}">
   <dimension ref="B1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="9"/>
       <c r="D1" s="1"/>
-      <c r="H1" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="H1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="8"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>62</v>
+      <c r="I3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="C7" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="I7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="C10" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="C11" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="I11" s="3" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C15" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="3" t="s">
+      <c r="C16" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="J29" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="J30" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C31" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="C32" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H25" s="5" t="s">
+      <c r="C33" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="I33" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H35" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I35" s="9"/>
-      <c r="J35" s="6" t="s">
-        <v>150</v>
+      <c r="H35" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1592,7 +2598,7 @@
   <dimension ref="B2:AK34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,130 +2631,130 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:37" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="B2" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="2:37" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="L4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD4" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="AE4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG4" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="AH4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="W4" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="X4" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y4" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z4" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA4" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB4" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC4" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD4" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="AE4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF4" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG4" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="AH4" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI4" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ4" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK4" s="12" t="s">
-        <v>64</v>
+      <c r="AK4" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
+      <c r="C5" s="13" t="s">
+        <v>168</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1784,19 +2790,19 @@
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
-        <v>3</v>
+      <c r="B6" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1805,11 +2811,11 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -1834,19 +2840,19 @@
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>5</v>
+      <c r="B7" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1855,11 +2861,11 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -1878,7 +2884,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
       <c r="AE7" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
@@ -1888,15 +2894,15 @@
       <c r="AK7" s="3"/>
     </row>
     <row r="8" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>7</v>
+      <c r="B8" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1905,11 +2911,11 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -1932,24 +2938,24 @@
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
       <c r="AI8" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ8" s="3"/>
       <c r="AK8" s="3"/>
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>9</v>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1957,11 +2963,11 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -1988,14 +2994,14 @@
       <c r="AK9" s="3"/>
     </row>
     <row r="10" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>11</v>
+      <c r="B10" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -2026,14 +3032,14 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
     </row>
     <row r="11" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
-        <v>13</v>
+      <c r="B11" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -2068,35 +3074,35 @@
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
       <c r="AI11" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AJ11" s="3" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="AK11" s="3"/>
     </row>
     <row r="12" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>15</v>
+      <c r="B12" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -2119,7 +3125,7 @@
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
@@ -2128,27 +3134,27 @@
       <c r="AK12" s="3"/>
     </row>
     <row r="13" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>17</v>
+      <c r="B13" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -2174,20 +3180,20 @@
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ13" s="3"/>
       <c r="AK13" s="3"/>
     </row>
     <row r="14" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
-        <v>19</v>
+      <c r="B14" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2218,21 +3224,21 @@
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
       <c r="AI14" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ14" s="3"/>
       <c r="AK14" s="3"/>
     </row>
     <row r="15" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>21</v>
+      <c r="B15" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -2262,14 +3268,14 @@
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
       <c r="AI15" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ15" s="3"/>
       <c r="AK15" s="3"/>
     </row>
     <row r="16" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
-        <v>23</v>
+      <c r="B16" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2277,7 +3283,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -2306,20 +3312,20 @@
       <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
       <c r="AI16" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AJ16" s="3"/>
       <c r="AK16" s="3"/>
     </row>
     <row r="17" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
-        <v>25</v>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2328,15 +3334,15 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
@@ -2354,18 +3360,18 @@
       <c r="AE17" s="3"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="AH17" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AI17" s="3"/>
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
     </row>
     <row r="18" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
-        <v>27</v>
+      <c r="B18" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2374,7 +3380,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -2402,14 +3408,14 @@
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
       <c r="AI18" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ18" s="3"/>
       <c r="AK18" s="3"/>
     </row>
     <row r="19" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
-        <v>29</v>
+      <c r="B19" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2418,7 +3424,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2442,7 +3448,7 @@
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
@@ -2452,8 +3458,8 @@
       <c r="AK19" s="3"/>
     </row>
     <row r="20" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
-        <v>31</v>
+      <c r="B20" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2463,7 +3469,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -2490,14 +3496,14 @@
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
       <c r="AI20" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ20" s="3"/>
       <c r="AK20" s="3"/>
     </row>
     <row r="21" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>33</v>
+      <c r="B21" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2508,7 +3514,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -2534,20 +3540,20 @@
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
       <c r="AI21" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ21" s="3"/>
       <c r="AK21" s="3"/>
     </row>
     <row r="22" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
-        <v>35</v>
+      <c r="B22" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -2556,17 +3562,17 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
@@ -2584,24 +3590,24 @@
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
       <c r="AG22" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="AH22" s="3"/>
       <c r="AI22" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ22" s="3"/>
       <c r="AK22" s="3"/>
     </row>
     <row r="23" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
-        <v>26</v>
+      <c r="B23" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -2610,15 +3616,15 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
@@ -2636,18 +3642,18 @@
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
       <c r="AG23" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="AH23" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AI23" s="3"/>
       <c r="AJ23" s="3"/>
       <c r="AK23" s="3"/>
     </row>
     <row r="24" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
-        <v>38</v>
+      <c r="B24" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -2668,22 +3674,22 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="V24" s="3" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="X24" s="3" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="Z24" s="3" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
@@ -2693,21 +3699,21 @@
       <c r="AF24" s="3"/>
       <c r="AG24" s="3"/>
       <c r="AH24" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AI24" s="3"/>
       <c r="AJ24" s="3"/>
       <c r="AK24" s="3"/>
     </row>
     <row r="25" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
-        <v>40</v>
+      <c r="B25" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -2716,36 +3722,36 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="V25" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="X25" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Y25" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Z25" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
@@ -2754,20 +3760,20 @@
       <c r="AE25" s="3"/>
       <c r="AF25" s="3"/>
       <c r="AG25" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="AH25" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AI25" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ25" s="3"/>
       <c r="AK25" s="3"/>
     </row>
     <row r="26" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
-        <v>42</v>
+      <c r="B26" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2785,33 +3791,33 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="V26" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="W26" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="X26" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="Y26" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AA26" s="3" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="AB26" s="3" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
@@ -2819,23 +3825,23 @@
       <c r="AF26" s="3"/>
       <c r="AG26" s="3"/>
       <c r="AH26" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AI26" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AJ26" s="3"/>
       <c r="AK26" s="3"/>
     </row>
     <row r="27" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
-        <v>44</v>
+      <c r="B27" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -2844,64 +3850,64 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="V27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="X27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Y27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AA27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AB27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
       <c r="AE27" s="3"/>
       <c r="AF27" s="3"/>
       <c r="AG27" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="AH27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AI27" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3"/>
     </row>
     <row r="28" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
-        <v>46</v>
+      <c r="B28" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2919,63 +3925,63 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="T28" s="3"/>
       <c r="U28" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="X28" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AA28" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AB28" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AC28" s="3" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="AD28" s="3" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="AE28" s="3"/>
       <c r="AF28" s="3"/>
       <c r="AG28" s="3"/>
       <c r="AH28" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AI28" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ28" s="3"/>
       <c r="AK28" s="3"/>
     </row>
     <row r="29" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
-        <v>48</v>
+      <c r="B29" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -2984,68 +3990,68 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="P29" s="3"/>
       <c r="Q29" s="3" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="V29" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="X29" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="Y29" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AA29" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AB29" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
       <c r="AF29" s="3"/>
       <c r="AG29" s="3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="AH29" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AI29" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="AJ29" s="3"/>
       <c r="AK29" s="3"/>
     </row>
     <row r="30" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
-        <v>50</v>
+      <c r="B30" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -3054,11 +4060,11 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
@@ -3066,54 +4072,54 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
       <c r="U30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="V30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="X30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AA30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AB30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
       <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
       <c r="AG30" s="3" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="AH30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AI30" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ30" s="3"/>
       <c r="AK30" s="3"/>
     </row>
     <row r="31" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B31" s="13" t="s">
-        <v>52</v>
+      <c r="B31" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -3122,36 +4128,36 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="P31" s="3"/>
       <c r="Q31" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="V31" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="W31" s="3" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="X31" s="3" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="Y31" s="3" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="AA31" s="3"/>
       <c r="AB31" s="3"/>
@@ -3160,7 +4166,7 @@
       <c r="AE31" s="3"/>
       <c r="AF31" s="3"/>
       <c r="AG31" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
@@ -3168,14 +4174,14 @@
       <c r="AK31" s="3"/>
     </row>
     <row r="32" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="s">
-        <v>54</v>
+      <c r="B32" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -3184,18 +4190,18 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="P32" s="3"/>
       <c r="Q32" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -3206,17 +4212,17 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
       <c r="AA32" s="3" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="AB32" s="3" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AH32" s="3"/>
       <c r="AI32" s="3"/>
@@ -3224,14 +4230,14 @@
       <c r="AK32" s="3"/>
     </row>
     <row r="33" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
-        <v>56</v>
+      <c r="B33" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -3240,19 +4246,19 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="P33" s="3"/>
       <c r="Q33" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="R33" s="3"/>
       <c r="S33" s="3" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
@@ -3264,15 +4270,15 @@
       <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="3" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="AD33" s="3" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="AE33" s="3"/>
       <c r="AF33" s="3"/>
       <c r="AG33" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
@@ -3280,8 +4286,8 @@
       <c r="AK33" s="3"/>
     </row>
     <row r="34" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
-        <v>58</v>
+      <c r="B34" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -3294,42 +4300,42 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="N34" s="3"/>
       <c r="O34" s="3" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
       <c r="U34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="V34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Y34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Z34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AA34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AB34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
@@ -3337,10 +4343,10 @@
       <c r="AF34" s="3"/>
       <c r="AG34" s="3"/>
       <c r="AH34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AI34" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="AJ34" s="3"/>
       <c r="AK34" s="3"/>

</xml_diff>